<commit_message>
Atualização trabalho final 1 termo
Foi atualizado algumas planilhaspara melhor entendimento de suas funções e gravado os videos de explicações das planilhas para colocar no site
</commit_message>
<xml_diff>
--- a/Trabalhos/Trabalho excel planilhas/Planilhas/Media_de_alunos_aprovados_por_ano_TI.xlsx
+++ b/Trabalhos/Trabalho excel planilhas/Planilhas/Media_de_alunos_aprovados_por_ano_TI.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diegofarias\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD1EBE3-B0DC-4DF6-A19C-67FC36292EC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -58,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +121,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -151,11 +157,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -170,6 +191,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,7 +238,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -258,6 +282,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -266,26 +291,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -426,7 +431,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D2D6-45A3-9FF8-CA952ABA188F}"/>
             </c:ext>
@@ -564,7 +569,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D2D6-45A3-9FF8-CA952ABA188F}"/>
             </c:ext>
@@ -580,11 +585,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1493986111"/>
-        <c:axId val="1311511567"/>
+        <c:axId val="111203840"/>
+        <c:axId val="111205376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1493986111"/>
+        <c:axId val="111203840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,7 +632,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1311511567"/>
+        <c:crossAx val="111205376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -635,7 +640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1311511567"/>
+        <c:axId val="111205376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,7 +691,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1493986111"/>
+        <c:crossAx val="111203840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -700,6 +705,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1329,7 +1335,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7665C2EA-B58A-481C-BA08-BB4ABDB9CC92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7665C2EA-B58A-481C-BA08-BB4ABDB9CC92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1639,18 +1645,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1678,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="2">
         <f ca="1">TODAY()</f>
-        <v>45043</v>
+        <v>45070</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1688,13 +1694,13 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1712,14 +1718,14 @@
         <f ca="1">YEAR(D1)</f>
         <v>2023</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="11">
         <v>2009</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="11">
         <f>COUNTIF(B2:B999999,"2009")</f>
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="11">
         <f>COUNTIFS(B3:B999999,"2009", C3:C999999, "Aprovado")</f>
         <v>2</v>
       </c>
@@ -1734,14 +1740,14 @@
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="11">
         <v>2010</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <f>COUNTIF(B2:B999999,"2010")</f>
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="11">
         <f>COUNTIFS(B3:B999999,"2010", C3:C999999, "Aprovado")</f>
         <v>1</v>
       </c>
@@ -1757,14 +1763,14 @@
         <v>10</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="H5">
+      <c r="H5" s="11">
         <v>2011</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="11">
         <f>COUNTIF(B2:B999999,"2011")</f>
         <v>1</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="12">
         <f>COUNTIFS(B3:B999999,"2011", C3:C999999, "Aprovado")</f>
         <v>0</v>
       </c>
@@ -1779,14 +1785,14 @@
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="11">
         <v>2012</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="11">
         <f>COUNTIF(B2:B999999,"2012")</f>
         <v>2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="12">
         <f>COUNTIFS(B3:B999999,"2012", C3:C999999, "Aprovado")</f>
         <v>2</v>
       </c>
@@ -1802,14 +1808,14 @@
         <v>9</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="H7">
+      <c r="H7" s="11">
         <v>2013</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="11">
         <f>COUNTIF(B2:B999999,"2013")</f>
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="11">
         <f>COUNTIFS(B3:B999999,"2013", C3:C999999, "Aprovado")</f>
         <v>2</v>
       </c>
@@ -1825,14 +1831,14 @@
         <v>10</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="H8">
+      <c r="H8" s="11">
         <v>2014</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="11">
         <f>COUNTIF(B2:B999999,"2014")</f>
         <v>3</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="11">
         <f>COUNTIFS(B3:B999999,"20014", C3:C999999, "Aprovado")</f>
         <v>0</v>
       </c>
@@ -1847,14 +1853,14 @@
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>2015</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="11">
         <f>COUNTIF(B2:B999999,"2015")</f>
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="11">
         <f>COUNTIFS(B3:B999999,"2015", C3:C999999, "Aprovado")</f>
         <v>1</v>
       </c>
@@ -1869,14 +1875,14 @@
       <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="11">
         <v>2016</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="11">
         <f>COUNTIF(B2:B999999,"2016")</f>
         <v>2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="11">
         <f>COUNTIFS(B3:B999999,"2016", C3:C999999, "Aprovado")</f>
         <v>0</v>
       </c>
@@ -1891,14 +1897,14 @@
       <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="11">
         <v>2017</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="11">
         <f>COUNTIF(B2:B999999,"2017")</f>
         <v>2</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="11">
         <f>COUNTIFS(B3:B999999,"2017", C3:C999999, "Aprovado")</f>
         <v>1</v>
       </c>
@@ -1913,14 +1919,14 @@
       <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="11">
         <v>2018</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="11">
         <f>COUNTIF(B2:B999999,"2018")</f>
         <v>2</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="11">
         <f>COUNTIFS(B3:B999999,"2018", C3:C999999, "Aprovado")</f>
         <v>2</v>
       </c>
@@ -1935,14 +1941,14 @@
       <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="11">
         <v>2019</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="11">
         <f>COUNTIF(B2:B999999,"2019")</f>
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="11">
         <f>COUNTIFS(B3:B999999,"2019", C3:C999999, "Aprovado")</f>
         <v>0</v>
       </c>
@@ -1957,14 +1963,14 @@
       <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="11">
         <v>2020</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="11">
         <f>COUNTIF(B2:B999999,"2020")</f>
         <v>2</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="11">
         <f>COUNTIFS(B3:B999999,"2020", C3:C999999, "Aprovado")</f>
         <v>2</v>
       </c>
@@ -1979,14 +1985,14 @@
       <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="11">
         <v>2021</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="11">
         <f>COUNTIF(B2:B999999,"2021")</f>
         <v>3</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="11">
         <f>COUNTIFS(B3:B999999,"2021", C3:C999999, "Aprovado")</f>
         <v>1</v>
       </c>
@@ -2001,14 +2007,14 @@
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="11">
         <v>2022</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="12">
         <f>COUNTIF(B2:B999999,"2022")</f>
         <v>2</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="11">
         <f>COUNTIFS(B3:B999999,"2022", C3:C999999, "Aprovado")</f>
         <v>0</v>
       </c>
@@ -2023,14 +2029,14 @@
       <c r="C17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="11">
         <v>2023</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="11">
         <f>COUNTIF(B2:B999999,"2023")</f>
         <v>4</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="11">
         <f>COUNTIFS(B3:B999999,"2023", C3:C999999, "Aprovado")</f>
         <v>4</v>
       </c>

</xml_diff>